<commit_message>
chat bot selecting category, choosing the group, sening the 5 tasks
</commit_message>
<xml_diff>
--- a/messages.xlsx
+++ b/messages.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -438,13 +438,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="10.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="8.109375" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -1181,6 +1181,909 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2023-08-21</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>14:00:31</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Madina Amankeldinova</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>amankeldinovam</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>a,dls,dfs,d;l,x'sd,c</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>inknkn]</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>jnkn;n</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>jknl;</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>партнер #1</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2023-08-21</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>14:05:23</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Madina Amankeldinova</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>amankeldinovam</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Институт</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>ВУЗ</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>XcˀṢfd</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>dfvbsdv</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>sfbvxvc</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>sfvxcfv</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>xdfvxdfv</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>партнер #1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2023-08-21</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>14:22:15</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Madina Amankeldinova</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>amankeldinovam</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Group B</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>w;d,fs,d</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>sdfcvsdv</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>sdvsdv</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>партнер #3</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2023-08-21</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>14:25:09</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Madina Amankeldinova</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>amankeldinovam</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Group B</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>ijojojo</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>ipjlk</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>uobjb</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>ibkb</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>13000</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>партнер #3</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2023-08-21</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>14:26:43</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Madina Amankeldinova</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>amankeldinovam</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Group B</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Дддд</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Ддд</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Ддд</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Ддд</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Ддд</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>партнер #2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2023-08-21</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>14:28:42</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Madina Amankeldinova</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>amankeldinovam</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Group C</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Щщз</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Лл</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Лл</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>партнер #3</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2023-08-21</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>14:30:08</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Madina Amankeldinova</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>amankeldinovam</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Group C</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Зз</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Зз</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Зз</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Дд</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Дщз</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>партнер #2</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2023-08-21</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>14:31:50</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Madina Amankeldinova</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>amankeldinovam</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Group A</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Цдщцщк</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Дцдадп</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Цллапш</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Дцла</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Лцлал</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>партнер #3</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2023-08-21</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>14:35:06</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Madina Amankeldinova</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>amankeldinovam</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Group B</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Щщщщ</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Дддд</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Эээ</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Ввв</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Миол</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>партнер #2</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2023-08-21</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>15:04:53</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Madina Amankeldinova</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>amankeldinovam</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Group C</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Щщлл</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Дщз</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Жз</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Ьл</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2023-08-21</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>15:20:09</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Madina Amankeldinova</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>amankeldinovam</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Group C</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Шддддорпа</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Уруоко</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Уруру</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Уруи</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>партнер #3</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2023-08-21</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>15:31:37</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Madina Amankeldinova</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>amankeldinovam</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Group C</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Зазрззазу</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Дудапл</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Луклао</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Оуоапл</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2023-08-21</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>15:33:52</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Madina Amankeldinova</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>amankeldinovam</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Group B</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>sfhdcgn</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>sfgdgb</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>v xcdfv</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>dfbdxf</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>rghfg</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2023-08-21</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>15:37:44</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Madina Amankeldinova</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>amankeldinovam</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Group C</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Цзущадал</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Улаллп</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Лулплпь</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>